<commit_message>
industry plot using highcharter
</commit_message>
<xml_diff>
--- a/datasets/labor/labor_education_haryana.xlsx
+++ b/datasets/labor/labor_education_haryana.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\econ_gju\datasets\labor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Music\econ_gju\datasets\labor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FF1132-D024-4D7A-AC1F-C3EC8D6B13B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925E0C63-2196-49B3-8A34-E665420721A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-114" yWindow="-114" windowWidth="19704" windowHeight="10736" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,10 +99,10 @@
     <t>UR</t>
   </si>
   <si>
-    <t>variable</t>
+    <t>Variable</t>
   </si>
   <si>
-    <t>value</t>
+    <t>Value</t>
   </si>
 </sst>
 </file>

</xml_diff>